<commit_message>
correcting linearization/TM analysis in previous pipelines
</commit_message>
<xml_diff>
--- a/s100a11.xlsx
+++ b/s100a11.xlsx
@@ -744,7 +744,7 @@
         <v>96</v>
       </c>
       <c r="D2">
-        <v>-0.1340724481567284</v>
+        <v>0.8555357224099455</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -758,7 +758,7 @@
         <v>97</v>
       </c>
       <c r="D3">
-        <v>-0.14086760232559</v>
+        <v>0.848213882228657</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -772,7 +772,7 @@
         <v>98</v>
       </c>
       <c r="D4">
-        <v>-0.08722831162310896</v>
+        <v>0.9060107039344742</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -786,7 +786,7 @@
         <v>99</v>
       </c>
       <c r="D5">
-        <v>0.5468160337377694</v>
+        <v>1.589199230525287</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -800,7 +800,7 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>0.1463847880185172</v>
+        <v>1.157730935341372</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -814,7 +814,7 @@
         <v>101</v>
       </c>
       <c r="D7">
-        <v>0.05666347848023479</v>
+        <v>1.061055411435596</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -828,7 +828,7 @@
         <v>102</v>
       </c>
       <c r="D8">
-        <v>0.1029733401509518</v>
+        <v>1.110954706954798</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -842,7 +842,7 @@
         <v>103</v>
       </c>
       <c r="D9">
-        <v>0.2885715823907533</v>
+        <v>1.310938494494903</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -856,7 +856,7 @@
         <v>104</v>
       </c>
       <c r="D10">
-        <v>0.7592142532218575</v>
+        <v>1.818060236354863</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -870,7 +870,7 @@
         <v>105</v>
       </c>
       <c r="D11">
-        <v>2.02579058815157</v>
+        <v>3.182807712468562</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -884,7 +884,7 @@
         <v>106</v>
       </c>
       <c r="D12">
-        <v>-0.1415766208858726</v>
+        <v>0.8474499083062189</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -898,7 +898,7 @@
         <v>96</v>
       </c>
       <c r="D13">
-        <v>0.1125222965906882</v>
+        <v>1.121243794032502</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -912,7 +912,7 @@
         <v>97</v>
       </c>
       <c r="D14">
-        <v>-0.06160947788385451</v>
+        <v>0.9336152293960717</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -926,7 +926,7 @@
         <v>98</v>
       </c>
       <c r="D15">
-        <v>0.05645873093851861</v>
+        <v>1.060834794104377</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -940,7 +940,7 @@
         <v>99</v>
       </c>
       <c r="D16">
-        <v>0.2967792430895584</v>
+        <v>1.319782323259565</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -954,7 +954,7 @@
         <v>100</v>
       </c>
       <c r="D17">
-        <v>0.0981250712794528</v>
+        <v>1.105730653320269</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -968,7 +968,7 @@
         <v>101</v>
       </c>
       <c r="D18">
-        <v>-0.1337421666622887</v>
+        <v>0.8558916037125665</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -982,7 +982,7 @@
         <v>102</v>
       </c>
       <c r="D19">
-        <v>-0.1107311139106122</v>
+        <v>0.8806862215334594</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -996,7 +996,7 @@
         <v>103</v>
       </c>
       <c r="D20">
-        <v>0.02002623722901209</v>
+        <v>1.021578452052687</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1010,7 +1010,7 @@
         <v>104</v>
       </c>
       <c r="D21">
-        <v>0.9973893501544218</v>
+        <v>2.074696061174605</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1024,7 +1024,7 @@
         <v>105</v>
       </c>
       <c r="D22">
-        <v>2.940234401869751</v>
+        <v>4.16812920664359</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1038,7 +1038,7 @@
         <v>107</v>
       </c>
       <c r="D23">
-        <v>-0.1009284162251264</v>
+        <v>0.8912487171023624</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1052,7 +1052,7 @@
         <v>96</v>
       </c>
       <c r="D24">
-        <v>0.03166322771436714</v>
+        <v>1.034117414732207</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1066,7 +1066,7 @@
         <v>97</v>
       </c>
       <c r="D25">
-        <v>0.08744042785770989</v>
+        <v>1.094217853230089</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1080,7 +1080,7 @@
         <v>98</v>
       </c>
       <c r="D26">
-        <v>0.1440785328888112</v>
+        <v>1.15524592454436</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1094,7 +1094,7 @@
         <v>99</v>
       </c>
       <c r="D27">
-        <v>0.1421480718394166</v>
+        <v>1.153165835273591</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1108,7 +1108,7 @@
         <v>100</v>
       </c>
       <c r="D28">
-        <v>-0.04082417555555717</v>
+        <v>0.9560115809703952</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1122,7 +1122,7 @@
         <v>101</v>
       </c>
       <c r="D29">
-        <v>0.01308578710617292</v>
+        <v>1.014100054164601</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1136,7 +1136,7 @@
         <v>102</v>
       </c>
       <c r="D30">
-        <v>-0.161862688052254</v>
+        <v>0.8255914871419483</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1150,7 +1150,7 @@
         <v>103</v>
       </c>
       <c r="D31">
-        <v>0.3412044436209094</v>
+        <v>1.367650879326003</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1164,7 +1164,7 @@
         <v>104</v>
       </c>
       <c r="D32">
-        <v>0.358476845701591</v>
+        <v>1.386262049056519</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1178,7 +1178,7 @@
         <v>105</v>
       </c>
       <c r="D33">
-        <v>1.061011762564319</v>
+        <v>2.143249786967603</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1192,7 +1192,7 @@
         <v>108</v>
       </c>
       <c r="D34">
-        <v>-0.08641196117994931</v>
+        <v>0.906890328933143</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1206,7 +1206,7 @@
         <v>96</v>
       </c>
       <c r="D35">
-        <v>-0.115307178546305</v>
+        <v>0.8757554704291911</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1220,7 +1220,7 @@
         <v>97</v>
       </c>
       <c r="D36">
-        <v>0.04202994253637349</v>
+        <v>1.045287643875726</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1234,7 +1234,7 @@
         <v>98</v>
       </c>
       <c r="D37">
-        <v>0.1387411517725061</v>
+        <v>1.149494848034677</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1248,7 +1248,7 @@
         <v>99</v>
       </c>
       <c r="D38">
-        <v>0.04614038569793144</v>
+        <v>1.049716683623067</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1262,7 +1262,7 @@
         <v>100</v>
       </c>
       <c r="D39">
-        <v>0.1649385570726221</v>
+        <v>1.177722789594982</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1276,7 +1276,7 @@
         <v>101</v>
       </c>
       <c r="D40">
-        <v>0.1457147194885866</v>
+        <v>1.157008930429527</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1290,7 +1290,7 @@
         <v>102</v>
       </c>
       <c r="D41">
-        <v>0.1223781016118579</v>
+        <v>1.131863513236758</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1304,7 +1304,7 @@
         <v>103</v>
       </c>
       <c r="D42">
-        <v>0.1361561972433813</v>
+        <v>1.146709536109764</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1318,7 +1318,7 @@
         <v>104</v>
       </c>
       <c r="D43">
-        <v>0.5803136342876836</v>
+        <v>1.625293198607279</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1332,7 +1332,7 @@
         <v>105</v>
       </c>
       <c r="D44">
-        <v>1.439656049009881</v>
+        <v>2.551242436143486</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1346,7 +1346,7 @@
         <v>109</v>
       </c>
       <c r="D45">
-        <v>-0.2756341932791664</v>
+        <v>0.7030016594860402</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1360,7 +1360,7 @@
         <v>96</v>
       </c>
       <c r="D46">
-        <v>-0.0681311562310114</v>
+        <v>0.9265880618903709</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1374,7 +1374,7 @@
         <v>97</v>
       </c>
       <c r="D47">
-        <v>-0.2891939184309879</v>
+        <v>0.6883909327833573</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1388,7 +1388,7 @@
         <v>98</v>
       </c>
       <c r="D48">
-        <v>-0.1469551622849402</v>
+        <v>0.841654481218946</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1402,7 +1402,7 @@
         <v>99</v>
       </c>
       <c r="D49">
-        <v>-0.06735592677239988</v>
+        <v>0.9274233786556314</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1416,7 +1416,7 @@
         <v>100</v>
       </c>
       <c r="D50">
-        <v>0.0395451777434489</v>
+        <v>1.042610287299292</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1430,7 +1430,7 @@
         <v>101</v>
       </c>
       <c r="D51">
-        <v>-0.1715202902711205</v>
+        <v>0.8151853332528979</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1444,7 +1444,7 @@
         <v>102</v>
       </c>
       <c r="D52">
-        <v>0.1661514108311937</v>
+        <v>1.179029650508341</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1458,7 +1458,7 @@
         <v>103</v>
       </c>
       <c r="D53">
-        <v>0.04499310496242648</v>
+        <v>1.048480478236156</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1472,7 +1472,7 @@
         <v>104</v>
       </c>
       <c r="D54">
-        <v>0.2745695156883325</v>
+        <v>1.295851140763819</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1486,7 +1486,7 @@
         <v>105</v>
       </c>
       <c r="D55">
-        <v>1.524513224289693</v>
+        <v>2.64267681131653</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1500,7 +1500,7 @@
         <v>110</v>
       </c>
       <c r="D56">
-        <v>5.851532824050857</v>
+        <v>7.305079633011651</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1514,7 +1514,7 @@
         <v>96</v>
       </c>
       <c r="D57">
-        <v>-0.004171957801666681</v>
+        <v>0.995504677670617</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1528,7 +1528,7 @@
         <v>97</v>
       </c>
       <c r="D58">
-        <v>-0.1416311343167914</v>
+        <v>0.8473911695905104</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1542,7 +1542,7 @@
         <v>98</v>
       </c>
       <c r="D59">
-        <v>0.02424145367943864</v>
+        <v>1.026120385968033</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1556,7 +1556,7 @@
         <v>99</v>
       </c>
       <c r="D60">
-        <v>0.4075446682318096</v>
+        <v>1.439133072389058</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1570,7 +1570,7 @@
         <v>100</v>
       </c>
       <c r="D61">
-        <v>0.1477261797620466</v>
+        <v>1.159176297098082</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1584,7 +1584,7 @@
         <v>101</v>
       </c>
       <c r="D62">
-        <v>-0.006985402703183818</v>
+        <v>0.9924731652993209</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1598,7 +1598,7 @@
         <v>102</v>
       </c>
       <c r="D63">
-        <v>-0.1519204245838374</v>
+        <v>0.8363043661064302</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1612,7 +1612,7 @@
         <v>103</v>
       </c>
       <c r="D64">
-        <v>-0.246181609790406</v>
+        <v>0.7347370850366403</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1626,7 +1626,7 @@
         <v>104</v>
       </c>
       <c r="D65">
-        <v>0.2203134699352745</v>
+        <v>1.237389759903182</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1640,7 +1640,7 @@
         <v>105</v>
       </c>
       <c r="D66">
-        <v>0.6361064645590673</v>
+        <v>1.685410478709735</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1654,7 +1654,7 @@
         <v>111</v>
       </c>
       <c r="D67">
-        <v>3.896502337441859</v>
+        <v>5.198516571044264</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1668,7 +1668,7 @@
         <v>96</v>
       </c>
       <c r="D68">
-        <v>-0.4321737055557467</v>
+        <v>0.5343289167544399</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1682,7 +1682,7 @@
         <v>97</v>
       </c>
       <c r="D69">
-        <v>-0.2825615209772153</v>
+        <v>0.6955374011295555</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1696,7 +1696,7 @@
         <v>98</v>
       </c>
       <c r="D70">
-        <v>-0.05528036089989907</v>
+        <v>0.9404349102883102</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1710,7 +1710,7 @@
         <v>99</v>
       </c>
       <c r="D71">
-        <v>-0.09667488666762747</v>
+        <v>0.8958319337376975</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1724,7 +1724,7 @@
         <v>100</v>
       </c>
       <c r="D72">
-        <v>-0.1385725556983405</v>
+        <v>0.8506868157627231</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1738,7 +1738,7 @@
         <v>101</v>
       </c>
       <c r="D73">
-        <v>-0.2737774066713903</v>
+        <v>0.7050023638784721</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1752,7 +1752,7 @@
         <v>102</v>
       </c>
       <c r="D74">
-        <v>0.1047615448605936</v>
+        <v>1.112881513730636</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1766,7 +1766,7 @@
         <v>103</v>
       </c>
       <c r="D75">
-        <v>-0.1913915388470642</v>
+        <v>0.7937738828780951</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1780,7 +1780,7 @@
         <v>104</v>
       </c>
       <c r="D76">
-        <v>0.4542615764859357</v>
+        <v>1.48947096428974</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1794,7 +1794,7 @@
         <v>105</v>
       </c>
       <c r="D77">
-        <v>1.233684023156432</v>
+        <v>2.329305712172467</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1808,7 +1808,7 @@
         <v>112</v>
       </c>
       <c r="D78">
-        <v>3.404734626687955</v>
+        <v>4.668632407273869</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1822,7 +1822,7 @@
         <v>96</v>
       </c>
       <c r="D79">
-        <v>1.850228955960178</v>
+        <v>2.993638463187666</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1836,7 +1836,7 @@
         <v>97</v>
       </c>
       <c r="D80">
-        <v>-0.1393383137364209</v>
+        <v>0.8498617045388961</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1850,7 +1850,7 @@
         <v>98</v>
       </c>
       <c r="D81">
-        <v>0.09791170293824503</v>
+        <v>1.105500746999493</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1864,7 +1864,7 @@
         <v>99</v>
       </c>
       <c r="D82">
-        <v>0.0908953808215538</v>
+        <v>1.097940596350628</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1878,7 +1878,7 @@
         <v>100</v>
       </c>
       <c r="D83">
-        <v>-0.1451121461423526</v>
+        <v>0.8436403478103764</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1892,7 +1892,7 @@
         <v>101</v>
       </c>
       <c r="D84">
-        <v>-0.1323093585154195</v>
+        <v>0.857435467472111</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1906,7 +1906,7 @@
         <v>102</v>
       </c>
       <c r="D85">
-        <v>-0.01991802467738579</v>
+        <v>0.9785381479521001</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1920,7 +1920,7 @@
         <v>103</v>
       </c>
       <c r="D86">
-        <v>0.09535474060571847</v>
+        <v>1.102745596920025</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1934,7 +1934,7 @@
         <v>104</v>
       </c>
       <c r="D87">
-        <v>1.725255984706422</v>
+        <v>2.85897895440215</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1948,7 +1948,7 @@
         <v>105</v>
       </c>
       <c r="D88">
-        <v>0.6997070951677244</v>
+        <v>1.753940734414553</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1962,7 +1962,7 @@
         <v>113</v>
       </c>
       <c r="D89">
-        <v>4.971872400572323</v>
+        <v>6.357237556958606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>